<commit_message>
ajout despreaux et noverre
</commit_message>
<xml_diff>
--- a/suivi.xlsx
+++ b/suivi.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10412"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/obvil/Documents/GitHub/danse/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE18AB08-2BF6-BC44-B0E3-53FBDC417B24}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B190CE04-4988-644C-8D5E-656EB38DF6DE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16340" xr2:uid="{E7B017DD-029B-5B4F-9960-5F1739140CC3}"/>
   </bookViews>
@@ -202,7 +202,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -225,11 +225,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -242,6 +255,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -558,8 +572,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09FF6D46-C474-7943-A787-912A5678F283}">
   <dimension ref="A1:C42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -587,7 +601,9 @@
       <c r="B2" s="2">
         <v>1</v>
       </c>
-      <c r="C2" s="2"/>
+      <c r="C2" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
@@ -596,7 +612,9 @@
       <c r="B3" s="2">
         <v>1</v>
       </c>
-      <c r="C3" s="2"/>
+      <c r="C3" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
@@ -605,7 +623,9 @@
       <c r="B4" s="2">
         <v>1</v>
       </c>
-      <c r="C4" s="2"/>
+      <c r="C4" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
@@ -614,7 +634,9 @@
       <c r="B5" s="2">
         <v>1</v>
       </c>
-      <c r="C5" s="2"/>
+      <c r="C5" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
@@ -623,7 +645,9 @@
       <c r="B6" s="2">
         <v>1</v>
       </c>
-      <c r="C6" s="2"/>
+      <c r="C6" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
@@ -632,7 +656,9 @@
       <c r="B7" s="2">
         <v>1</v>
       </c>
-      <c r="C7" s="2"/>
+      <c r="C7" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
@@ -641,7 +667,9 @@
       <c r="B8" s="2">
         <v>1</v>
       </c>
-      <c r="C8" s="2"/>
+      <c r="C8" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
@@ -650,7 +678,9 @@
       <c r="B9" s="2">
         <v>1</v>
       </c>
-      <c r="C9" s="2"/>
+      <c r="C9" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
@@ -659,7 +689,9 @@
       <c r="B10" s="2">
         <v>1</v>
       </c>
-      <c r="C10" s="2"/>
+      <c r="C10" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
@@ -668,7 +700,9 @@
       <c r="B11" s="2">
         <v>1</v>
       </c>
-      <c r="C11" s="2"/>
+      <c r="C11" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
@@ -677,7 +711,9 @@
       <c r="B12" s="2">
         <v>1</v>
       </c>
-      <c r="C12" s="2"/>
+      <c r="C12" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
@@ -686,7 +722,9 @@
       <c r="B13" s="2">
         <v>1</v>
       </c>
-      <c r="C13" s="2"/>
+      <c r="C13" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
@@ -695,7 +733,9 @@
       <c r="B14" s="2">
         <v>1</v>
       </c>
-      <c r="C14" s="2"/>
+      <c r="C14" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
@@ -704,7 +744,9 @@
       <c r="B15" s="2">
         <v>1</v>
       </c>
-      <c r="C15" s="2"/>
+      <c r="C15" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
@@ -713,7 +755,9 @@
       <c r="B16" s="2">
         <v>1</v>
       </c>
-      <c r="C16" s="2"/>
+      <c r="C16" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
@@ -722,7 +766,9 @@
       <c r="B17" s="2">
         <v>1</v>
       </c>
-      <c r="C17" s="2"/>
+      <c r="C17" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
@@ -731,7 +777,9 @@
       <c r="B18" s="2">
         <v>1</v>
       </c>
-      <c r="C18" s="2"/>
+      <c r="C18" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
@@ -740,7 +788,9 @@
       <c r="B19" s="2">
         <v>1</v>
       </c>
-      <c r="C19" s="2"/>
+      <c r="C19" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
@@ -749,7 +799,9 @@
       <c r="B20" s="2">
         <v>1</v>
       </c>
-      <c r="C20" s="2"/>
+      <c r="C20" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
@@ -758,7 +810,9 @@
       <c r="B21" s="2">
         <v>1</v>
       </c>
-      <c r="C21" s="2"/>
+      <c r="C21" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
@@ -767,7 +821,9 @@
       <c r="B22" s="2">
         <v>1</v>
       </c>
-      <c r="C22" s="2"/>
+      <c r="C22" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
@@ -776,7 +832,9 @@
       <c r="B23" s="2">
         <v>1</v>
       </c>
-      <c r="C23" s="2"/>
+      <c r="C23" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
@@ -785,7 +843,9 @@
       <c r="B24" s="2">
         <v>1</v>
       </c>
-      <c r="C24" s="2"/>
+      <c r="C24" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
@@ -794,7 +854,9 @@
       <c r="B25" s="2">
         <v>1</v>
       </c>
-      <c r="C25" s="2"/>
+      <c r="C25" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
@@ -803,7 +865,9 @@
       <c r="B26" s="2">
         <v>1</v>
       </c>
-      <c r="C26" s="2"/>
+      <c r="C26" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
@@ -812,7 +876,9 @@
       <c r="B27" s="2">
         <v>1</v>
       </c>
-      <c r="C27" s="2"/>
+      <c r="C27" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
@@ -821,7 +887,9 @@
       <c r="B28" s="2">
         <v>1</v>
       </c>
-      <c r="C28" s="2"/>
+      <c r="C28" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
@@ -830,7 +898,9 @@
       <c r="B29" s="2">
         <v>1</v>
       </c>
-      <c r="C29" s="2"/>
+      <c r="C29" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
@@ -839,7 +909,9 @@
       <c r="B30" s="2">
         <v>1</v>
       </c>
-      <c r="C30" s="2"/>
+      <c r="C30" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
@@ -848,7 +920,9 @@
       <c r="B31" s="2">
         <v>1</v>
       </c>
-      <c r="C31" s="2"/>
+      <c r="C31" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
@@ -857,7 +931,9 @@
       <c r="B32" s="2">
         <v>1</v>
       </c>
-      <c r="C32" s="2"/>
+      <c r="C32" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
@@ -866,7 +942,9 @@
       <c r="B33" s="2">
         <v>1</v>
       </c>
-      <c r="C33" s="2"/>
+      <c r="C33" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
@@ -875,7 +953,9 @@
       <c r="B34" s="2">
         <v>1</v>
       </c>
-      <c r="C34" s="2"/>
+      <c r="C34" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
@@ -884,7 +964,9 @@
       <c r="B35" s="2">
         <v>1</v>
       </c>
-      <c r="C35" s="2"/>
+      <c r="C35" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
@@ -893,7 +975,9 @@
       <c r="B36" s="2">
         <v>1</v>
       </c>
-      <c r="C36" s="2"/>
+      <c r="C36" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
@@ -902,7 +986,9 @@
       <c r="B37" s="2">
         <v>1</v>
       </c>
-      <c r="C37" s="2"/>
+      <c r="C37" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
@@ -911,7 +997,9 @@
       <c r="B38" s="2">
         <v>1</v>
       </c>
-      <c r="C38" s="2"/>
+      <c r="C38" s="6">
+        <v>1</v>
+      </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
@@ -920,16 +1008,22 @@
       <c r="B39" s="2">
         <v>0</v>
       </c>
-      <c r="C39" s="2"/>
+      <c r="C39" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
         <v>40</v>
       </c>
       <c r="B40" s="2">
+        <f>SUM(B2:B38)</f>
         <v>37</v>
       </c>
-      <c r="C40" s="2"/>
+      <c r="C40" s="2">
+        <f>SUM(C2:C38)</f>
+        <v>37</v>
+      </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">

</xml_diff>

<commit_message>
ajout de 4 fichiers (briffault, ehrarrd, fuller, vieil-abonne) et màj fichier de suivi
</commit_message>
<xml_diff>
--- a/suivi.xlsx
+++ b/suivi.xlsx
@@ -1,22 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/obvil/Documents/GitHub/danse/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B190CE04-4988-644C-8D5E-656EB38DF6DE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A9D5327-E37F-6445-808E-92CE45B4E75D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16340" xr2:uid="{E7B017DD-029B-5B4F-9960-5F1739140CC3}"/>
+    <workbookView xWindow="10380" yWindow="460" windowWidth="23600" windowHeight="16340" xr2:uid="{E7B017DD-029B-5B4F-9960-5F1739140CC3}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
     <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029" iterateDelta="1E-4"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Feuil1!$A$1:$D$49</definedName>
+  </definedNames>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
   <si>
     <t>angiolini_dissertation-ballets-pantomimes.xml</t>
   </si>
@@ -158,6 +161,27 @@
   </si>
   <si>
     <t>fichiers valides</t>
+  </si>
+  <si>
+    <t>briffault_opera_1834.xml</t>
+  </si>
+  <si>
+    <t>ehrhard_fanny-elssler_1909.xml</t>
+  </si>
+  <si>
+    <t>fuller_quinze-ans-de-ma-vie_1908.xml</t>
+  </si>
+  <si>
+    <t>vieil-abonne_ces-demoiselles-de-l-opera_1887.xml</t>
+  </si>
+  <si>
+    <t>despreaux_art-de-la-danse_1806.xml</t>
+  </si>
+  <si>
+    <t>noverre_lettres-danse-02_1803.xml</t>
+  </si>
+  <si>
+    <t>noverre_lettres-danse-04_1804_orig.xml</t>
   </si>
 </sst>
 </file>
@@ -202,7 +226,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -238,24 +262,59 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -570,480 +629,564 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09FF6D46-C474-7943-A787-912A5678F283}">
-  <dimension ref="A1:C42"/>
+  <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="41" customWidth="1"/>
+    <col min="1" max="1" width="45.5" customWidth="1"/>
     <col min="2" max="2" width="16.1640625" customWidth="1"/>
     <col min="3" max="3" width="14.5" customWidth="1"/>
+    <col min="4" max="4" width="30.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="2" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2">
-        <v>1</v>
-      </c>
-      <c r="C2" s="2">
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="2">
-        <v>1</v>
-      </c>
-      <c r="C3" s="2">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="2">
-        <v>1</v>
-      </c>
-      <c r="C4" s="2">
+      <c r="B4" s="1">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="2">
-        <v>1</v>
-      </c>
-      <c r="C5" s="2">
+      <c r="B5" s="1">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="2">
-        <v>1</v>
-      </c>
-      <c r="C6" s="2">
+      <c r="B6" s="1">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" s="1">
+        <v>1</v>
+      </c>
+      <c r="C7" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="2">
-        <v>1</v>
-      </c>
-      <c r="C7" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
+      <c r="B8" s="1">
+        <v>1</v>
+      </c>
+      <c r="C8" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="2">
-        <v>1</v>
-      </c>
-      <c r="C8" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
+      <c r="B9" s="1">
+        <v>1</v>
+      </c>
+      <c r="C9" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="2">
-        <v>1</v>
-      </c>
-      <c r="C9" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
+      <c r="B10" s="1">
+        <v>1</v>
+      </c>
+      <c r="C10" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B11" s="1">
+        <v>1</v>
+      </c>
+      <c r="C11" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="2">
-        <v>1</v>
-      </c>
-      <c r="C10" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
+      <c r="B12" s="1">
+        <v>1</v>
+      </c>
+      <c r="C12" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="2">
-        <v>1</v>
-      </c>
-      <c r="C11" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
+      <c r="B13" s="1">
+        <v>1</v>
+      </c>
+      <c r="C13" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14" s="1">
+        <v>1</v>
+      </c>
+      <c r="C14" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B15" s="1">
+        <v>1</v>
+      </c>
+      <c r="C15" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="2">
-        <v>1</v>
-      </c>
-      <c r="C12" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
+      <c r="B16" s="1">
+        <v>1</v>
+      </c>
+      <c r="C16" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="2">
-        <v>1</v>
-      </c>
-      <c r="C13" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
+      <c r="B17" s="1">
+        <v>1</v>
+      </c>
+      <c r="C17" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="2">
-        <v>1</v>
-      </c>
-      <c r="C14" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
+      <c r="B18" s="1">
+        <v>1</v>
+      </c>
+      <c r="C18" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="2">
-        <v>1</v>
-      </c>
-      <c r="C15" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="s">
+      <c r="B19" s="1">
+        <v>1</v>
+      </c>
+      <c r="C19" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="2">
-        <v>1</v>
-      </c>
-      <c r="C16" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="2" t="s">
+      <c r="B20" s="1">
+        <v>1</v>
+      </c>
+      <c r="C20" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="2">
-        <v>1</v>
-      </c>
-      <c r="C17" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="2" t="s">
+      <c r="B21" s="1">
+        <v>1</v>
+      </c>
+      <c r="C21" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="2">
-        <v>1</v>
-      </c>
-      <c r="C18" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" s="2" t="s">
+      <c r="B22" s="1">
+        <v>1</v>
+      </c>
+      <c r="C22" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="2">
-        <v>1</v>
-      </c>
-      <c r="C19" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" s="2" t="s">
+      <c r="B23" s="1">
+        <v>1</v>
+      </c>
+      <c r="C23" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="2">
-        <v>1</v>
-      </c>
-      <c r="C20" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" s="2" t="s">
+      <c r="B24" s="1">
+        <v>1</v>
+      </c>
+      <c r="C24" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="2">
-        <v>1</v>
-      </c>
-      <c r="C21" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" s="2" t="s">
+      <c r="B25" s="1">
+        <v>1</v>
+      </c>
+      <c r="C25" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B22" s="2">
-        <v>1</v>
-      </c>
-      <c r="C22" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" s="2" t="s">
+      <c r="B26" s="1">
+        <v>1</v>
+      </c>
+      <c r="C26" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B23" s="2">
-        <v>1</v>
-      </c>
-      <c r="C23" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" s="2" t="s">
+      <c r="B27" s="1">
+        <v>1</v>
+      </c>
+      <c r="C27" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B24" s="2">
-        <v>1</v>
-      </c>
-      <c r="C24" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" s="2" t="s">
+      <c r="B28" s="1">
+        <v>1</v>
+      </c>
+      <c r="C28" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B25" s="2">
-        <v>1</v>
-      </c>
-      <c r="C25" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" s="2" t="s">
+      <c r="B29" s="1">
+        <v>1</v>
+      </c>
+      <c r="C29" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B26" s="2">
-        <v>1</v>
-      </c>
-      <c r="C26" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27" s="2" t="s">
+      <c r="B30" s="1">
+        <v>1</v>
+      </c>
+      <c r="C30" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B27" s="2">
-        <v>1</v>
-      </c>
-      <c r="C27" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28" s="2" t="s">
+      <c r="B31" s="1">
+        <v>1</v>
+      </c>
+      <c r="C31" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B28" s="2">
-        <v>1</v>
-      </c>
-      <c r="C28" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29" s="2" t="s">
+      <c r="B32" s="1">
+        <v>1</v>
+      </c>
+      <c r="C32" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B29" s="2">
-        <v>1</v>
-      </c>
-      <c r="C29" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A30" s="2" t="s">
+      <c r="B33" s="1">
+        <v>1</v>
+      </c>
+      <c r="C33" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B34" s="1">
+        <v>1</v>
+      </c>
+      <c r="C34" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B30" s="2">
-        <v>1</v>
-      </c>
-      <c r="C30" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A31" s="2" t="s">
+      <c r="B35" s="1">
+        <v>1</v>
+      </c>
+      <c r="C35" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B36" s="1">
+        <v>1</v>
+      </c>
+      <c r="C36" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B31" s="2">
-        <v>1</v>
-      </c>
-      <c r="C31" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A32" s="2" t="s">
+      <c r="B37" s="1">
+        <v>1</v>
+      </c>
+      <c r="C37" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B32" s="2">
-        <v>1</v>
-      </c>
-      <c r="C32" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A33" s="2" t="s">
+      <c r="B38" s="1">
+        <v>1</v>
+      </c>
+      <c r="C38" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B33" s="2">
-        <v>1</v>
-      </c>
-      <c r="C33" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A34" s="2" t="s">
+      <c r="B39" s="1">
+        <v>1</v>
+      </c>
+      <c r="C39" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B34" s="2">
-        <v>1</v>
-      </c>
-      <c r="C34" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A35" s="2" t="s">
+      <c r="B40" s="1">
+        <v>1</v>
+      </c>
+      <c r="C40" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B35" s="2">
-        <v>1</v>
-      </c>
-      <c r="C35" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A36" s="2" t="s">
+      <c r="B41" s="1">
+        <v>1</v>
+      </c>
+      <c r="C41" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B36" s="2">
-        <v>1</v>
-      </c>
-      <c r="C36" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A37" s="2" t="s">
+      <c r="B42" s="1">
+        <v>1</v>
+      </c>
+      <c r="C42" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B37" s="2">
-        <v>1</v>
-      </c>
-      <c r="C37" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A38" s="2" t="s">
+      <c r="B43" s="1">
+        <v>1</v>
+      </c>
+      <c r="C43" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B38" s="2">
-        <v>1</v>
-      </c>
-      <c r="C38" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A39" s="1" t="s">
+      <c r="B44" s="1">
+        <v>1</v>
+      </c>
+      <c r="C44" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B45" s="1">
+        <v>1</v>
+      </c>
+      <c r="C45" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B46" s="1">
+        <v>0</v>
+      </c>
+      <c r="C46" s="4">
+        <v>0</v>
+      </c>
+      <c r="D46" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B39" s="2">
-        <v>0</v>
-      </c>
-      <c r="C39" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A40" s="3" t="s">
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B47" s="1">
+        <f>SUM(B2:B45)</f>
+        <v>44</v>
+      </c>
+      <c r="C47" s="4">
+        <f>SUM(C2:C45)</f>
+        <v>44</v>
+      </c>
+      <c r="D47" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="B40" s="2">
-        <f>SUM(B2:B38)</f>
-        <v>37</v>
-      </c>
-      <c r="C40" s="2">
-        <f>SUM(C2:C38)</f>
-        <v>37</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A41" s="3" t="s">
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B48" s="1">
+        <v>1</v>
+      </c>
+      <c r="C48" s="1"/>
+      <c r="D48" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B41" s="2">
-        <v>6</v>
-      </c>
-      <c r="C41" s="4"/>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A42" s="3" t="s">
+    </row>
+    <row r="49" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B49" s="7">
+        <f>SUM(B46:B48)</f>
+        <v>45</v>
+      </c>
+      <c r="C49" s="1"/>
+      <c r="D49" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="B42" s="2">
-        <v>43</v>
-      </c>
-      <c r="C42" s="4"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:D49" xr:uid="{0DE785A9-B169-994E-9099-EB5BCE84447F}">
+    <sortState ref="A2:D49">
+      <sortCondition ref="A1:A49"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>